<commit_message>
Import data beres amnjinc
</commit_message>
<xml_diff>
--- a/public/QuestionData/ayam.xlsx
+++ b/public/QuestionData/ayam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC552ED0-F933-4CC8-9ED1-FC12962E813F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178F3EC-5645-4D89-A789-E2CF2A19994E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{959A027F-E952-4A3F-86B3-B8CE4AFC19FE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="7">
   <si>
     <t>ayam</t>
   </si>
@@ -106,6 +106,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>18449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1881188</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1351950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18BAB41E-C30E-DE6D-142D-9FC8FA801AC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2376487" y="399449"/>
+          <a:ext cx="1333501" cy="1333501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,12 +462,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5972D6F3-DBF1-4F7A-9842-0CCFAC148FCD}">
   <dimension ref="B1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -468,12 +524,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -548,5 +601,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>